<commit_message>
Updated documents and reporting
</commit_message>
<xml_diff>
--- a/docs/rate.xlsx
+++ b/docs/rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22e8633286bd19a7/Documents/dev/map-reduce/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEEA66C-240E-415F-84B8-80E6C416CF59}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58E394FC-6F4F-4C63-B0FC-323366CF7794}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9DF68624-D4B9-4083-BFAE-DE2CA7971FFA}"/>
   </bookViews>
@@ -812,28 +812,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.35E-2</c:v>
+                  <c:v>1.5299999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.67E-2</c:v>
+                  <c:v>1.38E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1285</c:v>
+                  <c:v>0.13320000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4245999999999999</c:v>
+                  <c:v>1.5338000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.126100000000001</c:v>
+                  <c:v>13.767399999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.43089999999999</c:v>
+                  <c:v>118.60570000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1071.1759999999999</c:v>
+                  <c:v>1022.258</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10521.43</c:v>
+                  <c:v>10462.210000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,28 +929,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3663000000000001</c:v>
+                  <c:v>0.96619999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9877</c:v>
+                  <c:v>1.0487</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7414999999999998</c:v>
+                  <c:v>1.3159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2688000000000001</c:v>
+                  <c:v>1.7806</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9638999999999998</c:v>
+                  <c:v>7.6591999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.898499999999999</c:v>
+                  <c:v>35.364199999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>302.37220000000002</c:v>
+                  <c:v>298.73950000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2888.817</c:v>
+                  <c:v>2982.2883000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,28 +1040,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.2095E-2</c:v>
+                  <c:v>1.3261E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8890000000000002E-3</c:v>
+                  <c:v>7.1809999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7912E-2</c:v>
+                  <c:v>7.8535000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66601100000000002</c:v>
+                  <c:v>0.75371299999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2155259999999997</c:v>
+                  <c:v>7.7903689999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.902839999999998</c:v>
+                  <c:v>66.46069</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>674.29329999999993</c:v>
+                  <c:v>660.08050000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6514.6869999999999</c:v>
+                  <c:v>9478.5969999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1151,28 +1151,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.438361</c:v>
+                  <c:v>1.6995840000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4013879999999999</c:v>
+                  <c:v>1.1212899999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.237943</c:v>
+                  <c:v>1.424477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.775776</c:v>
+                  <c:v>1.4679379999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2084380000000001</c:v>
+                  <c:v>4.5098760000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.817129999999999</c:v>
+                  <c:v>18.800899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>139.59014000000002</c:v>
+                  <c:v>142.20162999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1403.9939999999999</c:v>
+                  <c:v>1331.6327999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1676,28 +1676,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.29E-2</c:v>
+                  <c:v>1.4599999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.44E-2</c:v>
+                  <c:v>1.1299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10550000000000001</c:v>
+                  <c:v>0.10490000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1881999999999999</c:v>
+                  <c:v>1.2861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9671000000000003</c:v>
+                  <c:v>11.281599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.956099999999992</c:v>
+                  <c:v>95.121000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>858.75699999999995</c:v>
+                  <c:v>813.226</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8393.23</c:v>
+                  <c:v>8356.2000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1793,28 +1793,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3202</c:v>
+                  <c:v>0.89380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9008</c:v>
+                  <c:v>0.99609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6469999999999998</c:v>
+                  <c:v>1.2238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8342000000000001</c:v>
+                  <c:v>1.4469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8664999999999998</c:v>
+                  <c:v>3.1673999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3176000000000005</c:v>
+                  <c:v>5.5765000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.7303</c:v>
+                  <c:v>30.401800000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>269.84500000000003</c:v>
+                  <c:v>268.22629999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,28 +1904,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.2022E-2</c:v>
+                  <c:v>1.3178E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5300000000000002E-3</c:v>
+                  <c:v>6.7489999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4578999999999998E-2</c:v>
+                  <c:v>7.4660000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63259200000000004</c:v>
+                  <c:v>0.717862</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8655799999999996</c:v>
+                  <c:v>7.4469899999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.680300000000003</c:v>
+                  <c:v>63.239999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>641.65599999999995</c:v>
+                  <c:v>626.78700000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6182.04</c:v>
+                  <c:v>9150.2099999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,28 +2015,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.365645</c:v>
+                  <c:v>1.6184690000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.313445</c:v>
+                  <c:v>1.036511</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1269210000000003</c:v>
+                  <c:v>1.3197239999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.582541</c:v>
+                  <c:v>1.2970569999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0874199999999998</c:v>
+                  <c:v>3.3543050000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5528199999999996</c:v>
+                  <c:v>7.0670299999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.762840000000001</c:v>
+                  <c:v>30.019930000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>269.35199999999998</c:v>
+                  <c:v>252.33579999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4066,8 +4066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE75E16D-024E-4063-A895-F36D0968513C}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4173,78 +4173,78 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1.4999999999999999E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="C2">
-        <v>7.9000000000000008E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="D2">
-        <v>5.9999999999999995E-4</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="E2">
         <f>SUM(B2:C2)</f>
-        <v>2.29E-2</v>
+        <v>1.4599999999999998E-2</v>
       </c>
       <c r="F2">
         <f>SUM(B2:D2)</f>
-        <v>2.35E-2</v>
+        <v>1.5299999999999998E-2</v>
       </c>
       <c r="G2">
-        <v>0.21779999999999999</v>
+        <v>0.2147</v>
       </c>
       <c r="H2">
-        <v>1.1024</v>
+        <v>0.67910000000000004</v>
       </c>
       <c r="I2">
-        <v>4.5499999999999999E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="J2">
-        <v>5.9999999999999995E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="K2">
         <f>SUM(G2:H2)</f>
-        <v>1.3202</v>
+        <v>0.89380000000000004</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L9" si="0">SUM(G2:J2)</f>
-        <v>1.3663000000000001</v>
+        <v>0.96619999999999995</v>
       </c>
       <c r="M2">
-        <v>9.358E-3</v>
+        <v>1.1736E-2</v>
       </c>
       <c r="N2">
-        <v>2.6640000000000001E-3</v>
+        <v>1.4419999999999999E-3</v>
       </c>
       <c r="O2" s="2">
-        <v>7.2999999999999999E-5</v>
+        <v>8.2999999999999998E-5</v>
       </c>
       <c r="P2">
         <f>SUM(M2:N2)</f>
-        <v>1.2022E-2</v>
+        <v>1.3178E-2</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q9" si="1">SUM(M2:O2)</f>
-        <v>1.2095E-2</v>
+        <v>1.3261E-2</v>
       </c>
       <c r="R2">
-        <v>0.61881699999999995</v>
+        <v>0.52131899999999998</v>
       </c>
       <c r="S2">
-        <v>0.74682800000000005</v>
+        <v>1.0971500000000001</v>
       </c>
       <c r="T2">
-        <v>7.2486999999999996E-2</v>
+        <v>8.0784999999999996E-2</v>
       </c>
       <c r="U2">
-        <v>2.2900000000000001E-4</v>
+        <v>3.3E-4</v>
       </c>
       <c r="V2">
         <f>SUM(R2:S2)</f>
-        <v>1.365645</v>
+        <v>1.6184690000000002</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W9" si="2">SUM(R2:U2)</f>
-        <v>1.438361</v>
+        <v>1.6995840000000002</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.45">
@@ -4252,78 +4252,78 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>1.12E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="C3">
-        <v>3.2000000000000002E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="D3">
-        <v>2.3E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E9" si="3">SUM(B3:C3)</f>
-        <v>1.44E-2</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F9" si="4">SUM(B3:D3)</f>
-        <v>1.67E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="G3">
-        <v>0.3972</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="H3">
-        <v>1.5036</v>
+        <v>0.79710000000000003</v>
       </c>
       <c r="I3">
-        <v>8.2600000000000007E-2</v>
+        <v>4.9799999999999997E-2</v>
       </c>
       <c r="J3">
-        <v>4.3E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K9" si="5">SUM(G3:H3)</f>
-        <v>1.9008</v>
+        <v>0.99609999999999999</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>1.9877</v>
+        <v>1.0487</v>
       </c>
       <c r="M3">
-        <v>4.849E-3</v>
+        <v>4.986E-3</v>
       </c>
       <c r="N3">
-        <v>1.681E-3</v>
+        <v>1.763E-3</v>
       </c>
       <c r="O3">
-        <v>3.59E-4</v>
+        <v>4.3199999999999998E-4</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P9" si="6">SUM(M3:N3)</f>
-        <v>6.5300000000000002E-3</v>
+        <v>6.7489999999999998E-3</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>6.8890000000000002E-3</v>
+        <v>7.1809999999999999E-3</v>
       </c>
       <c r="R3">
-        <v>0.50535200000000002</v>
+        <v>0.44561600000000001</v>
       </c>
       <c r="S3">
-        <v>0.80809299999999995</v>
+        <v>0.59089499999999995</v>
       </c>
       <c r="T3">
-        <v>8.7070999999999996E-2</v>
+        <v>8.3520999999999998E-2</v>
       </c>
       <c r="U3">
-        <v>8.7200000000000005E-4</v>
+        <v>1.258E-3</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V9" si="7">SUM(R3:S3)</f>
-        <v>1.313445</v>
+        <v>1.036511</v>
       </c>
       <c r="W3">
         <f t="shared" si="2"/>
-        <v>1.4013879999999999</v>
+        <v>1.1212899999999999</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.45">
@@ -4331,78 +4331,78 @@
         <v>1000</v>
       </c>
       <c r="B4">
-        <v>6.9400000000000003E-2</v>
+        <v>8.5900000000000004E-2</v>
       </c>
       <c r="C4">
-        <v>3.61E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D4">
-        <v>2.3E-2</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="E4">
         <f t="shared" si="3"/>
-        <v>0.10550000000000001</v>
+        <v>0.10490000000000001</v>
       </c>
       <c r="F4">
         <f t="shared" si="4"/>
-        <v>0.1285</v>
+        <v>0.13320000000000001</v>
       </c>
       <c r="G4">
-        <v>0.2046</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="H4">
-        <v>1.4423999999999999</v>
+        <v>1.0247999999999999</v>
       </c>
       <c r="I4">
-        <v>7.2400000000000006E-2</v>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="J4">
-        <v>2.2100000000000002E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>1.6469999999999998</v>
+        <v>1.2238</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1.7414999999999998</v>
+        <v>1.3159999999999998</v>
       </c>
       <c r="M4">
-        <v>4.9600999999999999E-2</v>
+        <v>5.6697999999999998E-2</v>
       </c>
       <c r="N4">
-        <v>1.4978E-2</v>
+        <v>1.7961999999999999E-2</v>
       </c>
       <c r="O4">
-        <v>3.333E-3</v>
+        <v>3.875E-3</v>
       </c>
       <c r="P4">
         <f t="shared" si="6"/>
-        <v>6.4578999999999998E-2</v>
+        <v>7.4660000000000004E-2</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>6.7912E-2</v>
+        <v>7.8535000000000008E-2</v>
       </c>
       <c r="R4">
-        <v>0.861151</v>
+        <v>0.47459200000000001</v>
       </c>
       <c r="S4">
-        <v>1.2657700000000001</v>
+        <v>0.84513199999999999</v>
       </c>
       <c r="T4">
-        <v>0.10402400000000001</v>
+        <v>9.7727999999999995E-2</v>
       </c>
       <c r="U4">
-        <v>6.9979999999999999E-3</v>
+        <v>7.025E-3</v>
       </c>
       <c r="V4">
         <f t="shared" si="7"/>
-        <v>2.1269210000000003</v>
+        <v>1.3197239999999999</v>
       </c>
       <c r="W4">
         <f t="shared" si="2"/>
-        <v>2.237943</v>
+        <v>1.424477</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.45">
@@ -4410,78 +4410,78 @@
         <v>10000</v>
       </c>
       <c r="B5">
-        <v>0.76649999999999996</v>
+        <v>0.84370000000000001</v>
       </c>
       <c r="C5">
-        <v>0.42170000000000002</v>
+        <v>0.44240000000000002</v>
       </c>
       <c r="D5">
-        <v>0.2364</v>
+        <v>0.2477</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1.1881999999999999</v>
+        <v>1.2861</v>
       </c>
       <c r="F5">
         <f t="shared" si="4"/>
-        <v>1.4245999999999999</v>
+        <v>1.5338000000000001</v>
       </c>
       <c r="G5">
-        <v>0.21190000000000001</v>
+        <v>0.2001</v>
       </c>
       <c r="H5">
-        <v>1.6223000000000001</v>
+        <v>1.2468999999999999</v>
       </c>
       <c r="I5">
-        <v>0.21859999999999999</v>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J5">
-        <v>0.216</v>
+        <v>0.24779999999999999</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>1.8342000000000001</v>
+        <v>1.4469999999999998</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>2.2688000000000001</v>
+        <v>1.7806</v>
       </c>
       <c r="M5">
-        <v>0.47629500000000002</v>
+        <v>0.54696199999999995</v>
       </c>
       <c r="N5">
-        <v>0.15629699999999999</v>
+        <v>0.1709</v>
       </c>
       <c r="O5">
-        <v>3.3418999999999997E-2</v>
+        <v>3.5851000000000001E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
-        <v>0.63259200000000004</v>
+        <v>0.717862</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>0.66601100000000002</v>
+        <v>0.75371299999999997</v>
       </c>
       <c r="R5">
-        <v>0.56026100000000001</v>
+        <v>0.47682099999999999</v>
       </c>
       <c r="S5">
-        <v>1.0222800000000001</v>
+        <v>0.82023599999999997</v>
       </c>
       <c r="T5">
-        <v>0.123677</v>
+        <v>0.105322</v>
       </c>
       <c r="U5">
-        <v>6.9557999999999995E-2</v>
+        <v>6.5559000000000006E-2</v>
       </c>
       <c r="V5">
         <f t="shared" si="7"/>
-        <v>1.582541</v>
+        <v>1.2970569999999999</v>
       </c>
       <c r="W5">
         <f t="shared" si="2"/>
-        <v>1.775776</v>
+        <v>1.4679379999999997</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.45">
@@ -4489,78 +4489,78 @@
         <v>100000</v>
       </c>
       <c r="B6">
-        <v>7.7336</v>
+        <v>8.7974999999999994</v>
       </c>
       <c r="C6">
-        <v>2.2334999999999998</v>
+        <v>2.4841000000000002</v>
       </c>
       <c r="D6">
-        <v>2.1589999999999998</v>
+        <v>2.4857999999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>9.9671000000000003</v>
+        <v>11.281599999999999</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
-        <v>12.126100000000001</v>
+        <v>13.767399999999999</v>
       </c>
       <c r="G6">
-        <v>0.20050000000000001</v>
+        <v>0.22470000000000001</v>
       </c>
       <c r="H6">
-        <v>3.6659999999999999</v>
+        <v>2.9426999999999999</v>
       </c>
       <c r="I6">
-        <v>1.7498</v>
+        <v>2.0160999999999998</v>
       </c>
       <c r="J6">
-        <v>2.3475999999999999</v>
+        <v>2.4756999999999998</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>3.8664999999999998</v>
+        <v>3.1673999999999998</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>7.9638999999999998</v>
+        <v>7.6591999999999993</v>
       </c>
       <c r="M6">
-        <v>5.0404799999999996</v>
+        <v>5.46922</v>
       </c>
       <c r="N6">
-        <v>1.8250999999999999</v>
+        <v>1.97777</v>
       </c>
       <c r="O6">
-        <v>0.34994599999999998</v>
+        <v>0.34337899999999999</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
-        <v>6.8655799999999996</v>
+        <v>7.4469899999999996</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>7.2155259999999997</v>
+        <v>7.7903689999999992</v>
       </c>
       <c r="R6">
-        <v>0.44688</v>
+        <v>0.37850499999999998</v>
       </c>
       <c r="S6">
-        <v>4.6405399999999997</v>
+        <v>2.9758</v>
       </c>
       <c r="T6">
-        <v>0.425288</v>
+        <v>0.464864</v>
       </c>
       <c r="U6">
-        <v>0.69572999999999996</v>
+        <v>0.69070699999999996</v>
       </c>
       <c r="V6">
         <f t="shared" si="7"/>
-        <v>5.0874199999999998</v>
+        <v>3.3543050000000001</v>
       </c>
       <c r="W6">
         <f t="shared" si="2"/>
-        <v>6.2084380000000001</v>
+        <v>4.5098760000000002</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.45">
@@ -4568,78 +4568,78 @@
         <v>1000000</v>
       </c>
       <c r="B7">
-        <v>64.174099999999996</v>
+        <v>73.321100000000001</v>
       </c>
       <c r="C7">
-        <v>19.782</v>
+        <v>21.799900000000001</v>
       </c>
       <c r="D7">
-        <v>21.474799999999998</v>
+        <v>23.4847</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>83.956099999999992</v>
+        <v>95.121000000000009</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>105.43089999999999</v>
+        <v>118.60570000000001</v>
       </c>
       <c r="G7">
-        <v>0.43159999999999998</v>
+        <v>0.47810000000000002</v>
       </c>
       <c r="H7">
-        <v>6.8860000000000001</v>
+        <v>5.0983999999999998</v>
       </c>
       <c r="I7">
-        <v>4.6177000000000001</v>
+        <v>4.6943999999999999</v>
       </c>
       <c r="J7">
-        <v>23.963200000000001</v>
+        <v>25.093299999999999</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>7.3176000000000005</v>
+        <v>5.5765000000000002</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>35.898499999999999</v>
+        <v>35.364199999999997</v>
       </c>
       <c r="M7">
-        <v>46.968699999999998</v>
+        <v>46.990099999999998</v>
       </c>
       <c r="N7">
-        <v>15.711600000000001</v>
+        <v>16.2499</v>
       </c>
       <c r="O7">
-        <v>3.22254</v>
+        <v>3.2206899999999998</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
-        <v>62.680300000000003</v>
+        <v>63.239999999999995</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>65.902839999999998</v>
+        <v>66.46069</v>
       </c>
       <c r="R7">
-        <v>0.84784000000000004</v>
+        <v>1.00038</v>
       </c>
       <c r="S7">
-        <v>5.7049799999999999</v>
+        <v>6.0666500000000001</v>
       </c>
       <c r="T7">
-        <v>2.4126099999999999</v>
+        <v>5.2098500000000003</v>
       </c>
       <c r="U7">
-        <v>6.8517000000000001</v>
+        <v>6.5240200000000002</v>
       </c>
       <c r="V7">
         <f t="shared" si="7"/>
-        <v>6.5528199999999996</v>
+        <v>7.0670299999999999</v>
       </c>
       <c r="W7">
         <f t="shared" si="2"/>
-        <v>15.817129999999999</v>
+        <v>18.800899999999999</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.45">
@@ -4647,78 +4647,78 @@
         <v>10000000</v>
       </c>
       <c r="B8">
-        <v>634.95299999999997</v>
+        <v>624.23699999999997</v>
       </c>
       <c r="C8">
-        <v>223.804</v>
+        <v>188.989</v>
       </c>
       <c r="D8">
-        <v>212.41900000000001</v>
+        <v>209.03200000000001</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>858.75699999999995</v>
+        <v>813.226</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>1071.1759999999999</v>
+        <v>1022.258</v>
       </c>
       <c r="G8">
-        <v>1.5701000000000001</v>
+        <v>0.98419999999999996</v>
       </c>
       <c r="H8">
-        <v>29.1602</v>
+        <v>29.4176</v>
       </c>
       <c r="I8">
-        <v>40.905900000000003</v>
+        <v>42.903700000000001</v>
       </c>
       <c r="J8">
-        <v>230.73599999999999</v>
+        <v>225.434</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>30.7303</v>
+        <v>30.401800000000001</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>302.37220000000002</v>
+        <v>298.73950000000002</v>
       </c>
       <c r="M8">
-        <v>483.28699999999998</v>
+        <v>458.85199999999998</v>
       </c>
       <c r="N8">
-        <v>158.369</v>
+        <v>167.935</v>
       </c>
       <c r="O8">
-        <v>32.637300000000003</v>
+        <v>33.293500000000002</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>641.65599999999995</v>
+        <v>626.78700000000003</v>
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
-        <v>674.29329999999993</v>
+        <v>660.08050000000003</v>
       </c>
       <c r="R8">
-        <v>2.0986400000000001</v>
+        <v>2.84823</v>
       </c>
       <c r="S8">
-        <v>27.664200000000001</v>
+        <v>27.171700000000001</v>
       </c>
       <c r="T8">
-        <v>44.231900000000003</v>
+        <v>46.458199999999998</v>
       </c>
       <c r="U8">
-        <v>65.595399999999998</v>
+        <v>65.723500000000001</v>
       </c>
       <c r="V8">
         <f t="shared" si="7"/>
-        <v>29.762840000000001</v>
+        <v>30.019930000000002</v>
       </c>
       <c r="W8">
         <f t="shared" si="2"/>
-        <v>139.59014000000002</v>
+        <v>142.20162999999999</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.45">
@@ -4726,78 +4726,78 @@
         <v>100000000</v>
       </c>
       <c r="B9">
-        <v>6414.86</v>
+        <v>6345.27</v>
       </c>
       <c r="C9">
-        <v>1978.37</v>
+        <v>2010.93</v>
       </c>
       <c r="D9">
-        <v>2128.1999999999998</v>
+        <v>2106.0100000000002</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>8393.23</v>
+        <v>8356.2000000000007</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>10521.43</v>
+        <v>10462.210000000001</v>
       </c>
       <c r="G9">
-        <v>7.3479999999999999</v>
+        <v>7.2793000000000001</v>
       </c>
       <c r="H9">
-        <v>262.49700000000001</v>
+        <v>260.947</v>
       </c>
       <c r="I9">
-        <v>407.92200000000003</v>
+        <v>373.25200000000001</v>
       </c>
       <c r="J9">
-        <v>2211.0500000000002</v>
+        <v>2340.81</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>269.84500000000003</v>
+        <v>268.22629999999998</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>2888.817</v>
+        <v>2982.2883000000002</v>
       </c>
       <c r="M9">
-        <v>4622.03</v>
+        <v>4632.47</v>
       </c>
       <c r="N9">
-        <v>1560.01</v>
+        <v>4517.74</v>
       </c>
       <c r="O9">
-        <v>332.64699999999999</v>
+        <v>328.387</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
-        <v>6182.04</v>
+        <v>9150.2099999999991</v>
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>6514.6869999999999</v>
+        <v>9478.5969999999998</v>
       </c>
       <c r="R9">
-        <v>16.789000000000001</v>
+        <v>16.939800000000002</v>
       </c>
       <c r="S9">
-        <v>252.56299999999999</v>
+        <v>235.39599999999999</v>
       </c>
       <c r="T9">
-        <v>455.79399999999998</v>
+        <v>431.298</v>
       </c>
       <c r="U9">
-        <v>678.84799999999996</v>
+        <v>647.99900000000002</v>
       </c>
       <c r="V9">
         <f t="shared" si="7"/>
-        <v>269.35199999999998</v>
+        <v>252.33579999999998</v>
       </c>
       <c r="W9">
         <f t="shared" si="2"/>
-        <v>1403.9939999999999</v>
+        <v>1331.6327999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>